<commit_message>
Dividir input por tipo de dato para no guardar todo como texto
</commit_message>
<xml_diff>
--- a/code/input.xlsx
+++ b/code/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2fee13dea56e37a/Documents/.Workspaces/NAEVYS2 Workspace/NAEVYS/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104828395F4F825ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BBF2A3A-81D2-4E4C-8C72-B10CA0BE6913}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC104828395F4F825ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02568F5D-83C7-484C-8B2A-F223436051E8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,10 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +130,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,7 +402,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +437,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>5</v>
       </c>
       <c r="C2" s="1">
@@ -456,7 +461,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>6</v>
       </c>
       <c r="C3" s="1">
@@ -480,7 +485,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>43</v>
       </c>
       <c r="C4" s="1">
@@ -504,7 +509,7 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>48</v>
       </c>
       <c r="C5" s="1">
@@ -528,7 +533,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>6</v>
       </c>
       <c r="C6" s="1">
@@ -552,7 +557,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>8</v>
       </c>
       <c r="C7" s="1">

</xml_diff>